<commit_message>
Weekly update and formula getting fixed
</commit_message>
<xml_diff>
--- a/LIN_DB/SCORESWeek11.xlsx
+++ b/LIN_DB/SCORESWeek11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,10 +471,8 @@
           <t>Pittsburgh Steelers</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="B4" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -483,10 +481,8 @@
           <t>Cleveland Browns</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+      <c r="B5" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="6">
@@ -495,10 +491,8 @@
           <t>Tennessee Titans</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+      <c r="B6" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="7">
@@ -507,10 +501,8 @@
           <t>Jacksonville Jaguars</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
+      <c r="B7" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="8">
@@ -519,10 +511,8 @@
           <t>Arizona Cardinals</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B8" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="9">
@@ -531,10 +521,8 @@
           <t>Houston Texans</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="B9" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="10">
@@ -543,10 +531,8 @@
           <t>Dallas Cowboys</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
+      <c r="B10" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="11">
@@ -555,10 +541,8 @@
           <t>Carolina Panthers</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="B11" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -567,10 +551,8 @@
           <t>Los Angeles Chargers</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B12" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="13">
@@ -579,10 +561,8 @@
           <t>Green Bay Packers</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
+      <c r="B13" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="14">
@@ -591,10 +571,8 @@
           <t>Las Vegas Raiders</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+      <c r="B14" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="15">
@@ -603,10 +581,8 @@
           <t>Miami Dolphins</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B15" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="16">
@@ -615,10 +591,8 @@
           <t>New York Giants</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
+      <c r="B16" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="17">
@@ -627,10 +601,8 @@
           <t>Washington Commanders</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="B17" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="18">
@@ -639,10 +611,8 @@
           <t>Chicago Bears</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
+      <c r="B18" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="19">
@@ -651,10 +621,8 @@
           <t>Detroit Lions</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
+      <c r="B19" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="20">
@@ -663,10 +631,8 @@
           <t>Tampa Bay Buccaneers</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+      <c r="B20" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="21">
@@ -675,10 +641,8 @@
           <t>San Francisco 49ers</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
+      <c r="B21" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="22">
@@ -687,10 +651,8 @@
           <t>New York Jets</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="B22" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="23">
@@ -699,10 +661,8 @@
           <t>Buffalo Bills</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="B23" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="24">
@@ -711,10 +671,8 @@
           <t>Seattle Seahawks</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B24" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="25">
@@ -723,10 +681,8 @@
           <t>Los Angeles Rams</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
+      <c r="B25" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="26">
@@ -735,10 +691,8 @@
           <t>Minnesota Vikings</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B26" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="27">
@@ -747,9 +701,31 @@
           <t>Denver Broncos</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Philadelphia Eagles</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
         <is>
           <t>21</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Kansas City Chiefs</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>17</t>
         </is>
       </c>
     </row>

</xml_diff>